<commit_message>
fix the problem of excel location
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataShareSkill.xlsx
+++ b/MarsFramework/ExcelData/TestDataShareSkill.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3(standard sprint)\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPER\source\repos\piper9797\Skillwap_Test3\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1978C4-282C-43B3-836F-A275C34D5D7F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB679B74-C257-4841-8E71-7D14F9663F61}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>http://www.skillswap.pro/Home</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   <si>
     <t>Arts</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://192.168.99.100:5000/</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -570,19 +570,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.65" x14ac:dyDescent="0.45">
@@ -599,7 +599,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -622,19 +622,19 @@
     </row>
     <row r="2" spans="1:3" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{ABA42B06-F2C9-4938-B15D-C1E56E54E02F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
@@ -664,76 +664,76 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="H2" s="5">
         <v>43567</v>
@@ -742,7 +742,7 @@
         <v>43597</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="7">
         <v>0.75</v>
@@ -751,16 +751,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>